<commit_message>
Maj Plan d action
</commit_message>
<xml_diff>
--- a/Plan d'action.xlsx
+++ b/Plan d'action.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Macro tâche</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Tâche</t>
   </si>
   <si>
-    <t>Temps estimé</t>
-  </si>
-  <si>
     <t>Acteur</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Alvyn</t>
   </si>
   <si>
-    <t>Réalisation du MCD</t>
-  </si>
-  <si>
     <t>Partie catalogue</t>
   </si>
   <si>
@@ -84,18 +78,6 @@
     <t>Groupe de requête 3</t>
   </si>
   <si>
-    <t>2 heures</t>
-  </si>
-  <si>
-    <t>3 heures</t>
-  </si>
-  <si>
-    <t>1 heure</t>
-  </si>
-  <si>
-    <t>30 minutes</t>
-  </si>
-  <si>
     <t>Préparation du rapport</t>
   </si>
   <si>
@@ -120,17 +102,86 @@
     <t>Réalisation du power point</t>
   </si>
   <si>
-    <t>Jour de la soutenance</t>
-  </si>
-  <si>
     <t>partie utilisateur,transporteur,commande</t>
+  </si>
+  <si>
+    <t>Alvyn, Hugo</t>
+  </si>
+  <si>
+    <t>Assemblage final</t>
+  </si>
+  <si>
+    <t>Temps estimé (en heures)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total d'heure : </t>
+  </si>
+  <si>
+    <t>(doit être au alentour de 60 heures)</t>
+  </si>
+  <si>
+    <t>Hugo,Sarah,Alvyn</t>
+  </si>
+  <si>
+    <t>Détails</t>
+  </si>
+  <si>
+    <t>Faire la partie catalogue en MEA, comprends : produit, film, type de support(catégorie), type de produit (Neuf, Occasion), genre,casting : (acteur,realisateur)</t>
+  </si>
+  <si>
+    <t>Faire la partie MEA : utilisateur(client, administrateur), commandes, transporteur, statut de commande, colis (livraison)</t>
+  </si>
+  <si>
+    <t>Faire le MEA, gestion lettre d'informations, scénario de fidélité,évenement</t>
+  </si>
+  <si>
+    <t>Aggrégation des différentes partie ensemble</t>
+  </si>
+  <si>
+    <t>Création d'un jeux de donnée pour toute les tables (3 entrées par tables)</t>
+  </si>
+  <si>
+    <t>Génération du script SQL puis teste et ajustement (moteur InnoDB)</t>
+  </si>
+  <si>
+    <t>Hugo -&gt; Faire liste de requete</t>
+  </si>
+  <si>
+    <t>Réalisation des différentes pages du rapport</t>
+  </si>
+  <si>
+    <t>Réalisation du MEA</t>
+  </si>
+  <si>
+    <t>Plan d'action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numéro de groupe : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chef de projet : </t>
+  </si>
+  <si>
+    <t>Hugo Poissonnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipe : </t>
+  </si>
+  <si>
+    <t>Sarah Villard, Hugo Poissonnet, Alvyn Silou</t>
+  </si>
+  <si>
+    <t>Version 1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0&quot; heures&quot;"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,16 +189,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -207,33 +286,384 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="3" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="3" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="3" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="3" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color theme="3" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="3" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="3" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="3" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="3" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -537,300 +967,465 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection sqref="A1:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="60">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="6">
+        <v>41256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G3" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="26">
+        <v>1</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="E4" s="9">
+        <v>41233</v>
+      </c>
+      <c r="F4" s="16">
+        <v>41256</v>
+      </c>
+      <c r="G4" s="35"/>
+    </row>
+    <row r="5" spans="1:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20"/>
+      <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="C5" s="27">
+        <v>1</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="19">
         <v>41233</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F5" s="19">
         <v>41256</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="5" t="s">
+      <c r="G5" s="31"/>
+    </row>
+    <row r="6" spans="1:7" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="28">
+        <v>3</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="17">
+        <v>41256</v>
+      </c>
+      <c r="F6" s="17">
+        <v>41263</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="29">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4">
-        <v>41233</v>
-      </c>
-      <c r="F3" s="4">
+      <c r="E7" s="2">
         <v>41256</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="F7" s="2">
+        <v>41263</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C8" s="29">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2">
+        <v>41256</v>
+      </c>
+      <c r="F8" s="2">
+        <v>41263</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="56"/>
+      <c r="B9" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="49">
+        <v>2</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="51">
+        <v>41263</v>
+      </c>
+      <c r="F9" s="51">
+        <v>41266</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B10" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="52">
+        <v>3</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="57">
+        <v>41266</v>
+      </c>
+      <c r="F10" s="57">
+        <v>41269</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="56"/>
+      <c r="B11" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="49">
+        <v>1</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="51">
+        <v>41269</v>
+      </c>
+      <c r="F11" s="51">
+        <v>41275</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="52">
+        <v>4</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="57">
+        <v>41275</v>
+      </c>
+      <c r="F12" s="57">
+        <v>41284</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="29">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="2">
+        <v>41275</v>
+      </c>
+      <c r="F13" s="2">
+        <v>41284</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21"/>
+      <c r="B14" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="27">
+        <v>4</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="19">
+        <v>41275</v>
+      </c>
+      <c r="F14" s="19">
+        <v>41284</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="30">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="9">
+        <v>41284</v>
+      </c>
+      <c r="F15" s="7">
+        <v>41289</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="29">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2">
+        <v>41284</v>
+      </c>
+      <c r="F16" s="33">
+        <v>41289</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="4">
-        <v>41256</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="4">
-        <v>41281</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="C17" s="29">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2">
+        <v>41284</v>
+      </c>
+      <c r="F17" s="34">
+        <v>41289</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="29">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2">
+        <v>41284</v>
+      </c>
+      <c r="F18" s="34">
+        <v>41289</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="56"/>
+      <c r="B19" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="49">
+        <v>2</v>
+      </c>
+      <c r="D19" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="E19" s="51">
+        <v>41284</v>
+      </c>
+      <c r="F19" s="58">
+        <v>41289</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B20" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="C20" s="43">
+        <v>3</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="45">
+        <v>41289</v>
+      </c>
+      <c r="F20" s="46">
+        <v>41295</v>
+      </c>
+      <c r="G20" s="32"/>
+    </row>
+    <row r="21" spans="1:7" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C21" s="30">
+        <f>SUM(C4:C20)</f>
+        <v>41</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A6:A9"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>